<commit_message>
Ward Locations Implemented :airplane:
Don't know why that needed an aircraft!
</commit_message>
<xml_diff>
--- a/server/CrimeData.xlsx
+++ b/server/CrimeData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="602">
   <si>
     <t>Abbey</t>
   </si>
@@ -1113,9 +1113,6 @@
     <t>Royal Hospital</t>
   </si>
   <si>
-    <t>St Helen's</t>
-  </si>
-  <si>
     <t>Stanley</t>
   </si>
   <si>
@@ -1621,12 +1618,6 @@
   </si>
   <si>
     <t>Bow West</t>
-  </si>
-  <si>
-    <t>Bromley North</t>
-  </si>
-  <si>
-    <t>Bromley South</t>
   </si>
   <si>
     <t>Canary Wharf</t>
@@ -2203,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="H355" sqref="H355"/>
+    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
+      <selection activeCell="S550" sqref="S550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5096,17 +5087,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A375" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B375" s="2">
-        <v>48</v>
-      </c>
-    </row>
+    <row r="375" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="376" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B376" s="2">
         <v>97</v>
@@ -5115,7 +5099,7 @@
     <row r="377" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="378" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B378" s="2">
         <v>22</v>
@@ -5123,7 +5107,7 @@
     </row>
     <row r="379" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B379" s="2">
         <v>53</v>
@@ -5131,7 +5115,7 @@
     </row>
     <row r="380" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B380" s="2">
         <v>47</v>
@@ -5139,7 +5123,7 @@
     </row>
     <row r="381" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B381" s="2">
         <v>58</v>
@@ -5147,7 +5131,7 @@
     </row>
     <row r="382" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B382" s="2">
         <v>38</v>
@@ -5155,7 +5139,7 @@
     </row>
     <row r="383" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B383" s="2">
         <v>40</v>
@@ -5163,7 +5147,7 @@
     </row>
     <row r="384" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B384" s="2">
         <v>22</v>
@@ -5171,7 +5155,7 @@
     </row>
     <row r="385" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B385" s="2">
         <v>267</v>
@@ -5179,7 +5163,7 @@
     </row>
     <row r="386" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B386" s="2">
         <v>72</v>
@@ -5187,7 +5171,7 @@
     </row>
     <row r="387" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B387" s="2">
         <v>23</v>
@@ -5195,7 +5179,7 @@
     </row>
     <row r="388" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B388" s="2">
         <v>24</v>
@@ -5203,7 +5187,7 @@
     </row>
     <row r="389" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B389" s="2">
         <v>66</v>
@@ -5211,7 +5195,7 @@
     </row>
     <row r="390" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B390" s="2">
         <v>29</v>
@@ -5219,7 +5203,7 @@
     </row>
     <row r="391" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B391" s="2">
         <v>45</v>
@@ -5227,7 +5211,7 @@
     </row>
     <row r="392" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B392" s="2">
         <v>35</v>
@@ -5235,7 +5219,7 @@
     </row>
     <row r="393" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B393" s="2">
         <v>255</v>
@@ -5243,7 +5227,7 @@
     </row>
     <row r="394" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B394" s="2">
         <v>131</v>
@@ -5251,7 +5235,7 @@
     </row>
     <row r="395" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B395" s="2">
         <v>125</v>
@@ -5259,7 +5243,7 @@
     </row>
     <row r="396" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B396" s="2">
         <v>182</v>
@@ -5267,7 +5251,7 @@
     </row>
     <row r="397" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B397" s="2">
         <v>302</v>
@@ -5275,7 +5259,7 @@
     </row>
     <row r="398" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B398" s="2">
         <v>138</v>
@@ -5283,7 +5267,7 @@
     </row>
     <row r="399" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B399" s="2">
         <v>103</v>
@@ -5291,7 +5275,7 @@
     </row>
     <row r="400" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B400" s="2">
         <v>129</v>
@@ -5299,7 +5283,7 @@
     </row>
     <row r="401" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B401" s="2">
         <v>82</v>
@@ -5307,7 +5291,7 @@
     </row>
     <row r="402" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B402" s="2">
         <v>139</v>
@@ -5315,7 +5299,7 @@
     </row>
     <row r="403" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B403" s="2">
         <v>164</v>
@@ -5323,7 +5307,7 @@
     </row>
     <row r="404" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B404" s="2">
         <v>141</v>
@@ -5331,7 +5315,7 @@
     </row>
     <row r="405" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B405" s="2">
         <v>138</v>
@@ -5339,7 +5323,7 @@
     </row>
     <row r="406" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B406" s="2">
         <v>108</v>
@@ -5347,7 +5331,7 @@
     </row>
     <row r="407" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B407" s="2">
         <v>86</v>
@@ -5355,7 +5339,7 @@
     </row>
     <row r="408" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B408" s="2">
         <v>91</v>
@@ -5363,7 +5347,7 @@
     </row>
     <row r="409" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B409" s="2">
         <v>85</v>
@@ -5371,7 +5355,7 @@
     </row>
     <row r="410" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B410" s="2">
         <v>67</v>
@@ -5379,7 +5363,7 @@
     </row>
     <row r="411" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B411" s="2">
         <v>71</v>
@@ -5387,7 +5371,7 @@
     </row>
     <row r="412" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B412" s="2">
         <v>110</v>
@@ -5395,7 +5379,7 @@
     </row>
     <row r="413" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B413" s="2">
         <v>105</v>
@@ -5403,7 +5387,7 @@
     </row>
     <row r="414" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B414" s="2">
         <v>106</v>
@@ -5411,7 +5395,7 @@
     </row>
     <row r="415" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B415" s="2">
         <v>103</v>
@@ -5419,7 +5403,7 @@
     </row>
     <row r="416" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B416" s="2">
         <v>132</v>
@@ -5427,7 +5411,7 @@
     </row>
     <row r="417" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B417" s="2">
         <v>65</v>
@@ -5435,7 +5419,7 @@
     </row>
     <row r="418" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B418" s="2">
         <v>63</v>
@@ -5443,7 +5427,7 @@
     </row>
     <row r="419" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B419" s="2">
         <v>107</v>
@@ -5451,7 +5435,7 @@
     </row>
     <row r="420" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B420" s="2">
         <v>114</v>
@@ -5459,7 +5443,7 @@
     </row>
     <row r="421" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B421" s="2">
         <v>107</v>
@@ -5467,7 +5451,7 @@
     </row>
     <row r="422" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B422" s="2">
         <v>69</v>
@@ -5475,7 +5459,7 @@
     </row>
     <row r="423" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B423" s="2">
         <v>87</v>
@@ -5483,7 +5467,7 @@
     </row>
     <row r="424" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B424" s="2">
         <v>88</v>
@@ -5491,7 +5475,7 @@
     </row>
     <row r="425" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B425" s="2">
         <v>283</v>
@@ -5499,7 +5483,7 @@
     </row>
     <row r="426" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B426" s="2">
         <v>157</v>
@@ -5507,7 +5491,7 @@
     </row>
     <row r="427" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B427" s="2">
         <v>111</v>
@@ -5515,7 +5499,7 @@
     </row>
     <row r="428" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B428" s="2">
         <v>178</v>
@@ -5523,7 +5507,7 @@
     </row>
     <row r="429" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B429" s="2">
         <v>74</v>
@@ -5531,7 +5515,7 @@
     </row>
     <row r="430" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B430" s="2">
         <v>96</v>
@@ -5539,7 +5523,7 @@
     </row>
     <row r="431" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B431" s="2">
         <v>92</v>
@@ -5548,7 +5532,7 @@
     <row r="432" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="433" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B433" s="2">
         <v>27</v>
@@ -5556,7 +5540,7 @@
     </row>
     <row r="434" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B434" s="2">
         <v>65</v>
@@ -5564,7 +5548,7 @@
     </row>
     <row r="435" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B435" s="2">
         <v>76</v>
@@ -5572,7 +5556,7 @@
     </row>
     <row r="436" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B436" s="2">
         <v>51</v>
@@ -5580,7 +5564,7 @@
     </row>
     <row r="437" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B437" s="2">
         <v>68</v>
@@ -5589,7 +5573,7 @@
     <row r="438" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="439" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B439" s="2">
         <v>43</v>
@@ -5597,7 +5581,7 @@
     </row>
     <row r="440" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B440" s="2">
         <v>58</v>
@@ -5605,7 +5589,7 @@
     </row>
     <row r="441" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B441" s="2">
         <v>39</v>
@@ -5613,7 +5597,7 @@
     </row>
     <row r="442" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B442" s="2">
         <v>21</v>
@@ -5621,7 +5605,7 @@
     </row>
     <row r="443" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B443" s="2">
         <v>36</v>
@@ -5629,7 +5613,7 @@
     </row>
     <row r="444" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B444" s="2">
         <v>42</v>
@@ -5637,7 +5621,7 @@
     </row>
     <row r="445" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B445" s="2">
         <v>70</v>
@@ -5645,7 +5629,7 @@
     </row>
     <row r="446" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B446" s="2">
         <v>38</v>
@@ -5653,7 +5637,7 @@
     </row>
     <row r="447" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B447" s="2">
         <v>47</v>
@@ -5661,7 +5645,7 @@
     </row>
     <row r="448" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B448" s="2">
         <v>80</v>
@@ -5670,7 +5654,7 @@
     <row r="449" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="450" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B450" s="2">
         <v>45</v>
@@ -5678,7 +5662,7 @@
     </row>
     <row r="451" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B451" s="2">
         <v>63</v>
@@ -5686,7 +5670,7 @@
     </row>
     <row r="452" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B452" s="2">
         <v>135</v>
@@ -5694,7 +5678,7 @@
     </row>
     <row r="453" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B453" s="2">
         <v>76</v>
@@ -5702,7 +5686,7 @@
     </row>
     <row r="454" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B454" s="2">
         <v>143</v>
@@ -5710,7 +5694,7 @@
     </row>
     <row r="455" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B455" s="2">
         <v>102</v>
@@ -5718,7 +5702,7 @@
     </row>
     <row r="456" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B456" s="2">
         <v>118</v>
@@ -5726,7 +5710,7 @@
     </row>
     <row r="457" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B457" s="2">
         <v>156</v>
@@ -5734,7 +5718,7 @@
     </row>
     <row r="458" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B458" s="2">
         <v>70</v>
@@ -5742,7 +5726,7 @@
     </row>
     <row r="459" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B459" s="2">
         <v>88</v>
@@ -5750,7 +5734,7 @@
     </row>
     <row r="460" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B460" s="2">
         <v>101</v>
@@ -5758,7 +5742,7 @@
     </row>
     <row r="461" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B461" s="2">
         <v>141</v>
@@ -5766,7 +5750,7 @@
     </row>
     <row r="462" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B462" s="2">
         <v>70</v>
@@ -5774,7 +5758,7 @@
     </row>
     <row r="463" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B463" s="2">
         <v>88</v>
@@ -5782,7 +5766,7 @@
     </row>
     <row r="464" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B464" s="2">
         <v>142</v>
@@ -5790,7 +5774,7 @@
     </row>
     <row r="465" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B465" s="2">
         <v>100</v>
@@ -5798,7 +5782,7 @@
     </row>
     <row r="466" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B466" s="2">
         <v>72</v>
@@ -5806,7 +5790,7 @@
     </row>
     <row r="467" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B467" s="2">
         <v>129</v>
@@ -5814,7 +5798,7 @@
     </row>
     <row r="468" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B468" s="2">
         <v>75</v>
@@ -5822,7 +5806,7 @@
     </row>
     <row r="469" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B469" s="2">
         <v>489</v>
@@ -5830,7 +5814,7 @@
     </row>
     <row r="470" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B470" s="2">
         <v>58</v>
@@ -5838,7 +5822,7 @@
     </row>
     <row r="471" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B471" s="2">
         <v>112</v>
@@ -5846,7 +5830,7 @@
     </row>
     <row r="472" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B472" s="2">
         <v>102</v>
@@ -5854,7 +5838,7 @@
     </row>
     <row r="473" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B473" s="2">
         <v>56</v>
@@ -5862,7 +5846,7 @@
     </row>
     <row r="474" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B474" s="2">
         <v>63</v>
@@ -5870,7 +5854,7 @@
     </row>
     <row r="475" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B475" s="2">
         <v>62</v>
@@ -5878,7 +5862,7 @@
     </row>
     <row r="476" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B476" s="2">
         <v>54</v>
@@ -5886,7 +5870,7 @@
     </row>
     <row r="477" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B477" s="2">
         <v>61</v>
@@ -5894,7 +5878,7 @@
     </row>
     <row r="478" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B478" s="2">
         <v>170</v>
@@ -5902,7 +5886,7 @@
     </row>
     <row r="479" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B479" s="2">
         <v>72</v>
@@ -5910,7 +5894,7 @@
     </row>
     <row r="480" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B480" s="2">
         <v>69</v>
@@ -5918,7 +5902,7 @@
     </row>
     <row r="481" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B481" s="2">
         <v>59</v>
@@ -5926,7 +5910,7 @@
     </row>
     <row r="482" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B482" s="2">
         <v>88</v>
@@ -5934,7 +5918,7 @@
     </row>
     <row r="483" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B483" s="2">
         <v>72</v>
@@ -5942,7 +5926,7 @@
     </row>
     <row r="484" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B484" s="2">
         <v>124</v>
@@ -5950,7 +5934,7 @@
     </row>
     <row r="485" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B485" s="2">
         <v>74</v>
@@ -5958,7 +5942,7 @@
     </row>
     <row r="486" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B486" s="2">
         <v>44</v>
@@ -5966,7 +5950,7 @@
     </row>
     <row r="487" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A487" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B487" s="2">
         <v>101</v>
@@ -5974,7 +5958,7 @@
     </row>
     <row r="488" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A488" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B488" s="2">
         <v>48</v>
@@ -5982,7 +5966,7 @@
     </row>
     <row r="489" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A489" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B489" s="2">
         <v>134</v>
@@ -5990,7 +5974,7 @@
     </row>
     <row r="490" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B490" s="2">
         <v>55</v>
@@ -5998,7 +5982,7 @@
     </row>
     <row r="491" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B491" s="2">
         <v>128</v>
@@ -6006,7 +5990,7 @@
     </row>
     <row r="492" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B492" s="2">
         <v>75</v>
@@ -6014,7 +5998,7 @@
     </row>
     <row r="493" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B493" s="2">
         <v>55</v>
@@ -6022,7 +6006,7 @@
     </row>
     <row r="494" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A494" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B494" s="2">
         <v>44</v>
@@ -6030,7 +6014,7 @@
     </row>
     <row r="495" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A495" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B495" s="2">
         <v>26</v>
@@ -6038,7 +6022,7 @@
     </row>
     <row r="496" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A496" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B496" s="2">
         <v>41</v>
@@ -6046,7 +6030,7 @@
     </row>
     <row r="497" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A497" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B497" s="2">
         <v>37</v>
@@ -6054,7 +6038,7 @@
     </row>
     <row r="498" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A498" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B498" s="2">
         <v>54</v>
@@ -6062,7 +6046,7 @@
     </row>
     <row r="499" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A499" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B499" s="2">
         <v>44</v>
@@ -6071,7 +6055,7 @@
     <row r="500" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="501" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A501" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B501" s="2">
         <v>59</v>
@@ -6079,7 +6063,7 @@
     </row>
     <row r="502" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A502" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B502" s="2">
         <v>60</v>
@@ -6087,7 +6071,7 @@
     </row>
     <row r="503" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A503" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B503" s="2">
         <v>56</v>
@@ -6095,7 +6079,7 @@
     </row>
     <row r="504" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A504" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B504" s="2">
         <v>44</v>
@@ -6103,7 +6087,7 @@
     </row>
     <row r="505" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A505" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B505" s="2">
         <v>79</v>
@@ -6111,7 +6095,7 @@
     </row>
     <row r="506" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A506" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B506" s="2">
         <v>40</v>
@@ -6119,7 +6103,7 @@
     </row>
     <row r="507" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A507" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B507" s="2">
         <v>52</v>
@@ -6127,7 +6111,7 @@
     </row>
     <row r="508" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A508" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B508" s="2">
         <v>52</v>
@@ -6135,7 +6119,7 @@
     </row>
     <row r="509" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A509" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B509" s="2">
         <v>45</v>
@@ -6143,7 +6127,7 @@
     </row>
     <row r="510" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A510" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B510" s="2">
         <v>43</v>
@@ -6159,7 +6143,7 @@
     </row>
     <row r="512" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A512" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B512" s="2">
         <v>144</v>
@@ -6167,7 +6151,7 @@
     </row>
     <row r="513" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A513" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B513" s="2">
         <v>256</v>
@@ -6175,7 +6159,7 @@
     </row>
     <row r="514" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A514" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B514" s="2">
         <v>176</v>
@@ -6183,7 +6167,7 @@
     </row>
     <row r="515" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A515" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B515" s="2">
         <v>104</v>
@@ -6191,7 +6175,7 @@
     </row>
     <row r="516" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A516" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B516" s="2">
         <v>55</v>
@@ -6199,7 +6183,7 @@
     </row>
     <row r="517" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A517" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B517" s="2">
         <v>148</v>
@@ -6207,7 +6191,7 @@
     </row>
     <row r="518" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A518" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B518" s="2">
         <v>100</v>
@@ -6223,7 +6207,7 @@
     </row>
     <row r="520" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A520" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B520" s="2">
         <v>125</v>
@@ -6231,7 +6215,7 @@
     </row>
     <row r="521" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A521" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B521" s="2">
         <v>152</v>
@@ -6239,7 +6223,7 @@
     </row>
     <row r="522" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A522" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B522" s="2">
         <v>110</v>
@@ -6247,7 +6231,7 @@
     </row>
     <row r="523" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A523" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B523" s="2">
         <v>108</v>
@@ -6255,7 +6239,7 @@
     </row>
     <row r="524" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A524" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B524" s="2">
         <v>77</v>
@@ -6263,7 +6247,7 @@
     </row>
     <row r="525" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A525" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B525" s="2">
         <v>146</v>
@@ -6271,7 +6255,7 @@
     </row>
     <row r="526" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A526" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B526" s="2">
         <v>130</v>
@@ -6279,7 +6263,7 @@
     </row>
     <row r="527" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A527" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B527" s="2">
         <v>126</v>
@@ -6287,7 +6271,7 @@
     </row>
     <row r="528" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A528" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B528" s="2">
         <v>64</v>
@@ -6295,7 +6279,7 @@
     </row>
     <row r="529" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A529" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B529" s="2">
         <v>87</v>
@@ -6303,7 +6287,7 @@
     </row>
     <row r="530" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A530" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B530" s="2">
         <v>214</v>
@@ -6312,7 +6296,7 @@
     <row r="531" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="532" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A532" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B532" s="2">
         <v>49</v>
@@ -6320,7 +6304,7 @@
     </row>
     <row r="533" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A533" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B533" s="2">
         <v>62</v>
@@ -6329,7 +6313,7 @@
     <row r="534" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="535" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A535" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B535" s="2">
         <v>47</v>
@@ -6337,7 +6321,7 @@
     </row>
     <row r="536" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A536" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B536" s="2">
         <v>43</v>
@@ -6345,7 +6329,7 @@
     </row>
     <row r="537" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A537" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B537" s="2">
         <v>44</v>
@@ -6353,7 +6337,7 @@
     </row>
     <row r="538" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A538" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B538" s="2">
         <v>37</v>
@@ -6362,7 +6346,7 @@
     <row r="539" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="540" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A540" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B540" s="2">
         <v>35</v>
@@ -6370,7 +6354,7 @@
     </row>
     <row r="541" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A541" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B541" s="2">
         <v>159</v>
@@ -6378,7 +6362,7 @@
     </row>
     <row r="542" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A542" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B542" s="2">
         <v>48</v>
@@ -6386,7 +6370,7 @@
     </row>
     <row r="543" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A543" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B543" s="2">
         <v>53</v>
@@ -6394,7 +6378,7 @@
     </row>
     <row r="544" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A544" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B544" s="2">
         <v>30</v>
@@ -6402,7 +6386,7 @@
     </row>
     <row r="545" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A545" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B545" s="2">
         <v>53</v>
@@ -6410,7 +6394,7 @@
     </row>
     <row r="546" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A546" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B546" s="2">
         <v>48</v>
@@ -6418,7 +6402,7 @@
     </row>
     <row r="547" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A547" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B547" s="2">
         <v>54</v>
@@ -6426,7 +6410,7 @@
     </row>
     <row r="548" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B548" s="2">
         <v>66</v>
@@ -6434,7 +6418,7 @@
     </row>
     <row r="549" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A549" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B549" s="2">
         <v>41</v>
@@ -6442,7 +6426,7 @@
     </row>
     <row r="550" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A550" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B550" s="2">
         <v>156</v>
@@ -6450,7 +6434,7 @@
     </row>
     <row r="551" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A551" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B551" s="2">
         <v>79</v>
@@ -6458,7 +6442,7 @@
     </row>
     <row r="552" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A552" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B552" s="2">
         <v>130</v>
@@ -6466,31 +6450,17 @@
     </row>
     <row r="553" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A553" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B553" s="2">
         <v>121</v>
       </c>
     </row>
-    <row r="554" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A554" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="B554" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="555" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A555" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="B555" s="2">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="554" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="555" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="556" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A556" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B556" s="2">
         <v>118</v>
@@ -6498,7 +6468,7 @@
     </row>
     <row r="557" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A557" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B557" s="2">
         <v>65</v>
@@ -6506,7 +6476,7 @@
     </row>
     <row r="558" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A558" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B558" s="2">
         <v>127</v>
@@ -6514,7 +6484,7 @@
     </row>
     <row r="559" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A559" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B559" s="2">
         <v>34</v>
@@ -6522,7 +6492,7 @@
     </row>
     <row r="560" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A560" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B560" s="2">
         <v>143</v>
@@ -6530,7 +6500,7 @@
     </row>
     <row r="561" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A561" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B561" s="2">
         <v>71</v>
@@ -6538,7 +6508,7 @@
     </row>
     <row r="562" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A562" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B562" s="2">
         <v>77</v>
@@ -6546,7 +6516,7 @@
     </row>
     <row r="563" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A563" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B563" s="2">
         <v>60</v>
@@ -6562,7 +6532,7 @@
     </row>
     <row r="565" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A565" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B565" s="2">
         <v>137</v>
@@ -6570,7 +6540,7 @@
     </row>
     <row r="566" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A566" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B566" s="2">
         <v>209</v>
@@ -6578,7 +6548,7 @@
     </row>
     <row r="567" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A567" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B567" s="2">
         <v>86</v>
@@ -6586,7 +6556,7 @@
     </row>
     <row r="568" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A568" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B568" s="2">
         <v>149</v>
@@ -6594,7 +6564,7 @@
     </row>
     <row r="569" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A569" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B569" s="2">
         <v>159</v>
@@ -6602,7 +6572,7 @@
     </row>
     <row r="570" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A570" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B570" s="2">
         <v>82</v>
@@ -6610,7 +6580,7 @@
     </row>
     <row r="571" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A571" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B571" s="2">
         <v>75</v>
@@ -6618,7 +6588,7 @@
     </row>
     <row r="572" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A572" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B572" s="2">
         <v>83</v>
@@ -6626,7 +6596,7 @@
     </row>
     <row r="573" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A573" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B573" s="2">
         <v>66</v>
@@ -6634,7 +6604,7 @@
     </row>
     <row r="574" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A574" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B574" s="2">
         <v>44</v>
@@ -6642,7 +6612,7 @@
     </row>
     <row r="575" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A575" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B575" s="2">
         <v>122</v>
@@ -6650,7 +6620,7 @@
     </row>
     <row r="576" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A576" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B576" s="2">
         <v>84</v>
@@ -6658,7 +6628,7 @@
     </row>
     <row r="577" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A577" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B577" s="2">
         <v>61</v>
@@ -6666,7 +6636,7 @@
     </row>
     <row r="578" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A578" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B578" s="2">
         <v>64</v>
@@ -6674,7 +6644,7 @@
     </row>
     <row r="579" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A579" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B579" s="2">
         <v>181</v>
@@ -6682,7 +6652,7 @@
     </row>
     <row r="580" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A580" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B580" s="2">
         <v>87</v>
@@ -6690,7 +6660,7 @@
     </row>
     <row r="581" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A581" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B581" s="2">
         <v>93</v>
@@ -6698,7 +6668,7 @@
     </row>
     <row r="582" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A582" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B582" s="2">
         <v>56</v>
@@ -6714,7 +6684,7 @@
     </row>
     <row r="584" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A584" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B584" s="2">
         <v>141</v>
@@ -6722,7 +6692,7 @@
     </row>
     <row r="585" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A585" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B585" s="2">
         <v>105</v>
@@ -6730,7 +6700,7 @@
     </row>
     <row r="586" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A586" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B586" s="2">
         <v>111</v>
@@ -6738,7 +6708,7 @@
     </row>
     <row r="587" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A587" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B587" s="2">
         <v>105</v>
@@ -6746,7 +6716,7 @@
     </row>
     <row r="588" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A588" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B588" s="2">
         <v>62</v>
@@ -6754,7 +6724,7 @@
     </row>
     <row r="589" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A589" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B589" s="2">
         <v>102</v>
@@ -6762,7 +6732,7 @@
     </row>
     <row r="590" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A590" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B590" s="2">
         <v>86</v>
@@ -6770,7 +6740,7 @@
     </row>
     <row r="591" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A591" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B591" s="2">
         <v>72</v>
@@ -6778,7 +6748,7 @@
     </row>
     <row r="592" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A592" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B592" s="2">
         <v>87</v>
@@ -6786,7 +6756,7 @@
     </row>
     <row r="593" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A593" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B593" s="2">
         <v>78</v>
@@ -6802,7 +6772,7 @@
     </row>
     <row r="595" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A595" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B595" s="2">
         <v>56</v>
@@ -6810,7 +6780,7 @@
     </row>
     <row r="596" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A596" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B596" s="2">
         <v>130</v>
@@ -6818,7 +6788,7 @@
     </row>
     <row r="597" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A597" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B597" s="2">
         <v>104</v>
@@ -6826,7 +6796,7 @@
     </row>
     <row r="598" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A598" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B598" s="2">
         <v>74</v>
@@ -6834,7 +6804,7 @@
     </row>
     <row r="599" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A599" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B599" s="2">
         <v>125</v>
@@ -6842,7 +6812,7 @@
     </row>
     <row r="600" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A600" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B600" s="2">
         <v>122</v>
@@ -6850,7 +6820,7 @@
     </row>
     <row r="601" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A601" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B601" s="2">
         <v>132</v>
@@ -6859,7 +6829,7 @@
     <row r="602" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="603" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A603" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B603" s="2">
         <v>73</v>
@@ -6867,7 +6837,7 @@
     </row>
     <row r="604" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A604" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B604" s="2">
         <v>103</v>
@@ -6875,7 +6845,7 @@
     </row>
     <row r="605" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A605" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B605" s="2">
         <v>131</v>
@@ -6883,7 +6853,7 @@
     </row>
     <row r="606" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A606" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B606" s="2">
         <v>96</v>
@@ -6891,7 +6861,7 @@
     </row>
     <row r="607" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A607" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B607" s="2">
         <v>72</v>
@@ -6899,7 +6869,7 @@
     </row>
     <row r="608" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A608" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B608" s="2">
         <v>76</v>
@@ -6907,7 +6877,7 @@
     </row>
     <row r="609" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A609" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B609" s="2">
         <v>86</v>
@@ -6915,7 +6885,7 @@
     </row>
     <row r="610" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A610" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B610" s="2">
         <v>54</v>
@@ -6923,7 +6893,7 @@
     </row>
     <row r="611" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A611" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B611" s="2">
         <v>91</v>
@@ -6931,7 +6901,7 @@
     </row>
     <row r="612" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A612" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B612" s="2">
         <v>156</v>
@@ -6939,7 +6909,7 @@
     </row>
     <row r="613" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A613" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B613" s="2">
         <v>84</v>
@@ -6947,7 +6917,7 @@
     </row>
     <row r="614" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A614" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B614" s="2">
         <v>90</v>
@@ -6955,7 +6925,7 @@
     </row>
     <row r="615" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A615" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B615" s="2">
         <v>82</v>
@@ -6963,7 +6933,7 @@
     </row>
     <row r="616" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A616" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B616" s="2">
         <v>178</v>
@@ -6971,7 +6941,7 @@
     </row>
     <row r="617" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A617" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B617" s="2">
         <v>172</v>
@@ -6979,7 +6949,7 @@
     </row>
     <row r="618" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A618" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B618" s="2">
         <v>158</v>
@@ -6987,7 +6957,7 @@
     </row>
     <row r="619" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A619" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B619" s="2">
         <v>67</v>
@@ -6995,7 +6965,7 @@
     </row>
     <row r="620" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A620" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B620" s="2">
         <v>57</v>
@@ -7003,7 +6973,7 @@
     </row>
     <row r="621" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A621" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B621" s="2">
         <v>268</v>
@@ -7011,7 +6981,7 @@
     </row>
     <row r="622" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A622" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B622" s="2">
         <v>71</v>
@@ -7027,7 +6997,7 @@
     </row>
     <row r="624" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A624" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B624" s="2">
         <v>825</v>
@@ -7035,7 +7005,7 @@
     </row>
     <row r="625" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A625" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B625" s="2">
         <v>48</v>
@@ -7043,7 +7013,7 @@
     </row>
     <row r="626" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A626" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B626" s="2">
         <v>82</v>
@@ -7051,7 +7021,7 @@
     </row>
     <row r="627" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A627" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B627" s="2">
         <v>92</v>
@@ -7059,7 +7029,7 @@
     </row>
     <row r="628" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A628" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B628" s="2">
         <v>75</v>
@@ -7067,7 +7037,7 @@
     </row>
     <row r="629" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A629" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B629" s="2">
         <v>1085</v>

</xml_diff>